<commit_message>
lrc vs rfc comparisons
</commit_message>
<xml_diff>
--- a/grp_data.xlsx
+++ b/grp_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtd28\Desktop\CSINTSY'\pinoybot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karl Divinagracia\Desktop\CSINTSY\pinoybot\pinoybot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75777492-1F42-494C-B818-2C0B6D91BEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F33C2C7-6B2D-4CC1-BF56-13CAC5B50CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3E369064-A925-42E2-ADF4-F15E5F9A959C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{AEDA3BCB-B6A2-4BE4-AD1C-918ABB9ECFC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -403,7 +401,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -415,7 +413,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -459,839 +457,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="208">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA9A9A9"/>
-          <bgColor rgb="FFA9A9A9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA9A9A9"/>
-          <bgColor rgb="FFA9A9A9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEDEDED"/>
-          <bgColor rgb="FFEDEDED"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDDEBF7"/>
-          <bgColor rgb="FFDDEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2F0D9"/>
-          <bgColor rgb="FFE2F0D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE4D6"/>
-          <bgColor rgb="FFFCE4D6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA9A9A9"/>
-          <bgColor rgb="FFA9A9A9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFDA"/>
-          <bgColor rgb="FFE2EFDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor rgb="FFD9D9D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4B084"/>
-          <bgColor rgb="FFF4B084"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFD966"/>
-          <bgColor rgb="FFFFD966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6E0B4"/>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB4C7E7"/>
-          <bgColor rgb="FFB4C7E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA9A9A9"/>
-          <bgColor rgb="FFA9A9A9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEDEDED"/>
-          <bgColor rgb="FFEDEDED"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDDEBF7"/>
-          <bgColor rgb="FFDDEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2F0D9"/>
-          <bgColor rgb="FFE2F0D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE4D6"/>
-          <bgColor rgb="FFFCE4D6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFDA"/>
-          <bgColor rgb="FFE2EFDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor rgb="FFD9D9D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4B084"/>
-          <bgColor rgb="FFF4B084"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFD966"/>
-          <bgColor rgb="FFFFD966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6E0B4"/>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB4C7E7"/>
-          <bgColor rgb="FFB4C7E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA9A9A9"/>
-          <bgColor rgb="FFA9A9A9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA9A9A9"/>
-          <bgColor rgb="FFA9A9A9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEDEDED"/>
-          <bgColor rgb="FFEDEDED"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDDEBF7"/>
-          <bgColor rgb="FFDDEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2F0D9"/>
-          <bgColor rgb="FFE2F0D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE4D6"/>
-          <bgColor rgb="FFFCE4D6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA9A9A9"/>
-          <bgColor rgb="FFA9A9A9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFDA"/>
-          <bgColor rgb="FFE2EFDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor rgb="FFD9D9D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4B084"/>
-          <bgColor rgb="FFF4B084"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFD966"/>
-          <bgColor rgb="FFFFD966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6E0B4"/>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB4C7E7"/>
-          <bgColor rgb="FFB4C7E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA9A9A9"/>
-          <bgColor rgb="FFA9A9A9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEDEDED"/>
-          <bgColor rgb="FFEDEDED"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDDEBF7"/>
-          <bgColor rgb="FFDDEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2F0D9"/>
-          <bgColor rgb="FFE2F0D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE4D6"/>
-          <bgColor rgb="FFFCE4D6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFDA"/>
-          <bgColor rgb="FFE2EFDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor rgb="FFD9D9D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4B084"/>
-          <bgColor rgb="FFF4B084"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFD966"/>
-          <bgColor rgb="FFFFD966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6E0B4"/>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB4C7E7"/>
-          <bgColor rgb="FFB4C7E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA9A9A9"/>
-          <bgColor rgb="FFA9A9A9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA9A9A9"/>
-          <bgColor rgb="FFA9A9A9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEDEDED"/>
-          <bgColor rgb="FFEDEDED"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDDEBF7"/>
-          <bgColor rgb="FFDDEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2F0D9"/>
-          <bgColor rgb="FFE2F0D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE4D6"/>
-          <bgColor rgb="FFFCE4D6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA9A9A9"/>
-          <bgColor rgb="FFA9A9A9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFDA"/>
-          <bgColor rgb="FFE2EFDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor rgb="FFD9D9D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4B084"/>
-          <bgColor rgb="FFF4B084"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFD966"/>
-          <bgColor rgb="FFFFD966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6E0B4"/>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB4C7E7"/>
-          <bgColor rgb="FFB4C7E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA9A9A9"/>
-          <bgColor rgb="FFA9A9A9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEDEDED"/>
-          <bgColor rgb="FFEDEDED"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDDEBF7"/>
-          <bgColor rgb="FFDDEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2F0D9"/>
-          <bgColor rgb="FFE2F0D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE4D6"/>
-          <bgColor rgb="FFFCE4D6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFDA"/>
-          <bgColor rgb="FFE2EFDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor rgb="FFD9D9D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4B084"/>
-          <bgColor rgb="FFF4B084"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFD966"/>
-          <bgColor rgb="FFFFD966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6E0B4"/>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB4C7E7"/>
-          <bgColor rgb="FFB4C7E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA9A9A9"/>
-          <bgColor rgb="FFA9A9A9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA9A9A9"/>
-          <bgColor rgb="FFA9A9A9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEDEDED"/>
-          <bgColor rgb="FFEDEDED"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDDEBF7"/>
-          <bgColor rgb="FFDDEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2F0D9"/>
-          <bgColor rgb="FFE2F0D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE4D6"/>
-          <bgColor rgb="FFFCE4D6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA9A9A9"/>
-          <bgColor rgb="FFA9A9A9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFDA"/>
-          <bgColor rgb="FFE2EFDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor rgb="FFD9D9D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4B084"/>
-          <bgColor rgb="FFF4B084"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFD966"/>
-          <bgColor rgb="FFFFD966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6E0B4"/>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB4C7E7"/>
-          <bgColor rgb="FFB4C7E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA9A9A9"/>
-          <bgColor rgb="FFA9A9A9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEDEDED"/>
-          <bgColor rgb="FFEDEDED"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDDEBF7"/>
-          <bgColor rgb="FFDDEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2F0D9"/>
-          <bgColor rgb="FFE2F0D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE4D6"/>
-          <bgColor rgb="FFFCE4D6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFDA"/>
-          <bgColor rgb="FFE2EFDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor rgb="FFD9D9D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4B084"/>
-          <bgColor rgb="FFF4B084"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFD966"/>
-          <bgColor rgb="FFFFD966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6E0B4"/>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB4C7E7"/>
-          <bgColor rgb="FFB4C7E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="104">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2148,39 +1314,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2232,7 +1398,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2343,6 +1509,13 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -2351,13 +1524,6 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -2422,47 +1588,30 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{183E6133-58F9-46FC-8E5D-DCDEE0653621}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF4BDC3-EB9B-44D6-8F5A-17BE85C2A846}">
   <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="V8" sqref="V8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="125.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>107</v>
       </c>
@@ -2500,7 +1649,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>155</v>
       </c>
@@ -2530,7 +1679,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>156</v>
       </c>
@@ -2558,7 +1707,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>157</v>
       </c>
@@ -2586,7 +1735,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>158</v>
       </c>
@@ -2614,7 +1763,7 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>159</v>
       </c>
@@ -2642,7 +1791,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>160</v>
       </c>
@@ -2670,7 +1819,7 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>161</v>
       </c>
@@ -2698,7 +1847,7 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>162</v>
       </c>
@@ -2726,7 +1875,7 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>163</v>
       </c>
@@ -2754,7 +1903,7 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>164</v>
       </c>
@@ -2782,7 +1931,7 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>165</v>
       </c>
@@ -2810,7 +1959,7 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>166</v>
       </c>
@@ -2838,7 +1987,7 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>167</v>
       </c>
@@ -2866,7 +2015,7 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>168</v>
       </c>
@@ -2896,7 +2045,7 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>169</v>
       </c>
@@ -2926,7 +2075,7 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>170</v>
       </c>
@@ -2954,7 +2103,7 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>171</v>
       </c>
@@ -2984,7 +2133,7 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>172</v>
       </c>
@@ -3014,7 +2163,7 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>173</v>
       </c>
@@ -3042,7 +2191,7 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>174</v>
       </c>
@@ -3070,7 +2219,7 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>175</v>
       </c>
@@ -3098,7 +2247,7 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>176</v>
       </c>
@@ -3128,7 +2277,7 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>177</v>
       </c>
@@ -3158,7 +2307,7 @@
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>178</v>
       </c>
@@ -3186,7 +2335,7 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>179</v>
       </c>
@@ -3214,7 +2363,7 @@
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>180</v>
       </c>
@@ -3242,7 +2391,7 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>181</v>
       </c>
@@ -3270,7 +2419,7 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>182</v>
       </c>
@@ -3298,7 +2447,7 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>183</v>
       </c>
@@ -3326,7 +2475,7 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>184</v>
       </c>
@@ -3353,7 +2502,7 @@
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
     </row>
-    <row r="32" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>185</v>
       </c>
@@ -3380,7 +2529,7 @@
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
     </row>
-    <row r="33" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>186</v>
       </c>
@@ -3407,7 +2556,7 @@
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
     </row>
-    <row r="34" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>187</v>
       </c>
@@ -3434,7 +2583,7 @@
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
     </row>
-    <row r="35" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>188</v>
       </c>
@@ -3461,7 +2610,7 @@
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
     </row>
-    <row r="36" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>189</v>
       </c>
@@ -3488,7 +2637,7 @@
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
     </row>
-    <row r="37" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>190</v>
       </c>
@@ -3515,7 +2664,7 @@
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
     </row>
-    <row r="38" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>191</v>
       </c>
@@ -3542,7 +2691,7 @@
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
     </row>
-    <row r="39" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>192</v>
       </c>
@@ -3571,7 +2720,7 @@
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
     </row>
-    <row r="40" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>193</v>
       </c>
@@ -3598,7 +2747,7 @@
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
     </row>
-    <row r="41" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>194</v>
       </c>
@@ -3625,7 +2774,7 @@
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
     </row>
-    <row r="42" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>195</v>
       </c>
@@ -3652,7 +2801,7 @@
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
     </row>
-    <row r="43" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>196</v>
       </c>
@@ -3679,7 +2828,7 @@
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
     </row>
-    <row r="44" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>197</v>
       </c>
@@ -3708,7 +2857,7 @@
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
     </row>
-    <row r="45" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>198</v>
       </c>
@@ -3736,7 +2885,7 @@
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
     </row>
-    <row r="46" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>199</v>
       </c>
@@ -3764,7 +2913,7 @@
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
     </row>
-    <row r="47" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>200</v>
       </c>
@@ -3792,7 +2941,7 @@
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
     </row>
-    <row r="48" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>201</v>
       </c>
@@ -3820,7 +2969,7 @@
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
     </row>
-    <row r="49" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>202</v>
       </c>
@@ -3848,7 +2997,7 @@
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
     </row>
-    <row r="50" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>203</v>
       </c>
@@ -3876,7 +3025,7 @@
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
     </row>
-    <row r="51" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>204</v>
       </c>
@@ -3904,7 +3053,7 @@
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
     </row>
-    <row r="52" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>205</v>
       </c>
@@ -3932,7 +3081,7 @@
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
     </row>
-    <row r="53" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>206</v>
       </c>
@@ -4052,13 +3201,13 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" sqref="H2:H53 K2:K53" xr:uid="{78DBD2FC-3CBA-494C-9501-043655643018}">
+    <dataValidation type="list" allowBlank="1" sqref="H2:H53 K2:K53" xr:uid="{043F8220-347E-4630-878C-B4B1926CB645}">
       <formula1>"T,F,TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="G2:G53 J2:J53" xr:uid="{407F9ED6-FD28-47E1-9DBE-392A9B794A92}">
+    <dataValidation type="list" allowBlank="1" sqref="G2:G53 J2:J53" xr:uid="{C0E83419-D6C7-4983-B665-FF0FB19D8EA8}">
       <formula1>"NE,ABB,EXPR,ABB_NE,ABB_EXPR"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F2:F53 I2:I53" xr:uid="{45343601-3271-4C8F-AAE7-9AE08AD1A4F7}">
+    <dataValidation type="list" allowBlank="1" sqref="F2:F53 I2:I53" xr:uid="{58033AC9-C1E9-48BE-974D-A49CEE085EEA}">
       <formula1>"FIL,ENG,CS,SYM,UNK,NUM"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>